<commit_message>
Charge pump and new area/PPA stuff
</commit_message>
<xml_diff>
--- a/figures/PPA.xlsx
+++ b/figures/PPA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://levylab-my.sharepoint.com/personal/akash_levy_365_levylab_org/Documents/Documents/Research/Writing/NEMS CGRA ASP-DAC 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akashlevy/Documents/NEM-Relay-CAD/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="8_{655A2804-2553-C043-94D4-54BC596DD0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE85A3A-8432-B14C-8348-EB73026C48E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBAEDEB-2174-AE4A-A2D9-6DB5DFBBBED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{4B8004C3-4F04-8948-99E3-8ED7038A9C13}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{4B8004C3-4F04-8948-99E3-8ED7038A9C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>CMOS</t>
   </si>
@@ -161,16 +161,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1377,15 +1377,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3180,10 +3180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951DB8D2-0273-2745-B4A8-72F558841444}">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3280,12 +3280,12 @@
       </c>
     </row>
     <row r="3" spans="1:24" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -3307,7 +3307,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -3362,7 +3362,7 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G9">
@@ -3371,7 +3371,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="7"/>
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -3394,7 +3394,7 @@
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="7"/>
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -3473,7 +3473,7 @@
         <f>X11-SUM(T11:V11)</f>
         <v>2.9125099999999959E-2</v>
       </c>
-      <c r="X11" s="7">
+      <c r="X11" s="4">
         <v>0.46050000000000002</v>
       </c>
     </row>
@@ -3512,12 +3512,12 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -3539,7 +3539,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="7"/>
       <c r="B24" t="s">
         <v>16</v>
       </c>
@@ -3584,12 +3584,12 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>15</v>
       </c>
@@ -3611,7 +3611,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>16</v>
       </c>
@@ -3632,8 +3632,84 @@
         <v>6.2836056528589881E-2</v>
       </c>
     </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="7"/>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="7"/>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="7"/>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A49:A51"/>
     <mergeCell ref="O1:S1"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="A25:A27"/>

</xml_diff>